<commit_message>
Updated roles list with turn order
</commit_message>
<xml_diff>
--- a/Roles.xlsx
+++ b/Roles.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Roles" sheetId="1" r:id="rId1"/>
+    <sheet name="Turn Order" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>Role</t>
   </si>
@@ -393,12 +393,36 @@
   <si>
     <t>Werewolf that wakes with other wolves. If killed, wolves kill two players the next night</t>
   </si>
+  <si>
+    <t>Turn Order</t>
+  </si>
+  <si>
+    <t>First Night</t>
+  </si>
+  <si>
+    <t>Masons</t>
+  </si>
+  <si>
+    <t>Subsiquent Nights</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>Bodyguard</t>
+  </si>
+  <si>
+    <t>Wolves</t>
+  </si>
+  <si>
+    <t>Vampires</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +441,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -444,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -457,6 +489,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,13 +1431,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A10:C10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>